<commit_message>
sửa export với import hóa đơn, voucher, thêm địa chỉ cho khách hàng nếu chưa cso địa chỉ
</commit_message>
<xml_diff>
--- a/src/main/resources/static/xuatExcel/danhSachHoaDon.xlsx
+++ b/src/main/resources/static/xuatExcel/danhSachHoaDon.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Admin\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Admin\Desktop\DATN\DATN_BE_2003Shoes\src\main\resources\static\xuatExcel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{62226E38-0B2C-4569-8C82-714D91171157}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA60365E-D954-44FC-A0B8-AE5E0E93A80F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{85EF4E9E-2678-4BFE-9A88-F9038E36C35E}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="10080" xr2:uid="{85EF4E9E-2678-4BFE-9A88-F9038E36C35E}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -69,6 +69,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="165" formatCode="[$-1010409]d/m/yyyy\ h:mm\ AM/PM;@"/>
+  </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -132,13 +135,17 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="165" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -458,7 +465,7 @@
   <dimension ref="A1:H3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+      <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
@@ -469,7 +476,7 @@
     <col min="4" max="4" width="21.6328125" style="1" customWidth="1"/>
     <col min="5" max="5" width="18.90625" style="1" customWidth="1"/>
     <col min="6" max="6" width="23.453125" style="1" customWidth="1"/>
-    <col min="7" max="7" width="30.90625" style="1" customWidth="1"/>
+    <col min="7" max="7" width="30.90625" style="4" customWidth="1"/>
     <col min="8" max="8" width="14.81640625" style="1" customWidth="1"/>
     <col min="9" max="16384" width="8.7265625" style="1"/>
   </cols>
@@ -498,7 +505,7 @@
       <c r="F3" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="G3" s="3" t="s">
+      <c r="G3" s="5" t="s">
         <v>7</v>
       </c>
       <c r="H3" s="3" t="s">

</xml_diff>